<commit_message>
bj: update oncho stop forms
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Benin/stop/bj_oncho_stop_6_202306_usage_facility.xlsx
+++ b/ONCHO/Impact Assessments/Benin/stop/bj_oncho_stop_6_202306_usage_facility.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Impact Assessments\Benin\stop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE47EADC-E5EA-4876-B28A-363911BD158C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E56CB0-CD20-4E4E-80F5-8AA5D05D4112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -116,9 +116,6 @@
     <t>bj_oncho_stop_6_202306_usage_facility</t>
   </si>
   <si>
-    <t>(2023 Juillet) ONCHO Stop TDM - 5. Questionnaire sur la facilité d'utilisation</t>
-  </si>
-  <si>
     <t>Appréciation globale</t>
   </si>
   <si>
@@ -417,6 +414,9 @@
   </si>
   <si>
     <t>Tout à fait d.accord</t>
+  </si>
+  <si>
+    <t>(2023 Juillet) ONCHO Stop TDM - 6. Questionnaire sur la facilité d'utilisation</t>
   </si>
 </sst>
 </file>
@@ -991,13 +991,13 @@
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="13"/>
@@ -1013,13 +1013,13 @@
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" s="20"/>
       <c r="E3" s="13"/>
@@ -1035,13 +1035,13 @@
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="15"/>
@@ -1057,13 +1057,13 @@
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="25"/>
       <c r="E5" s="26"/>
@@ -1077,13 +1077,13 @@
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>56</v>
-      </c>
       <c r="C6" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="15"/>
@@ -1099,13 +1099,13 @@
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="13"/>
@@ -1121,13 +1121,13 @@
     </row>
     <row r="8" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="15"/>
@@ -1143,13 +1143,13 @@
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="15"/>
@@ -1168,10 +1168,10 @@
         <v>17</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="13"/>
@@ -1190,10 +1190,10 @@
         <v>17</v>
       </c>
       <c r="B11" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="20" t="s">
         <v>66</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>67</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="13"/>
@@ -1208,13 +1208,13 @@
     </row>
     <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>68</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>69</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="26"/>
@@ -1228,13 +1228,13 @@
     </row>
     <row r="13" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="13"/>
@@ -1250,13 +1250,13 @@
     </row>
     <row r="14" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="13"/>
@@ -1271,13 +1271,13 @@
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" s="20"/>
       <c r="E15" s="13"/>
@@ -1292,13 +1292,13 @@
     </row>
     <row r="16" spans="1:12" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="13"/>
@@ -1314,13 +1314,13 @@
     </row>
     <row r="17" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="26"/>
@@ -1334,13 +1334,13 @@
     </row>
     <row r="18" spans="1:12" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="9"/>
@@ -1356,13 +1356,13 @@
     </row>
     <row r="19" spans="1:12" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D19" s="16"/>
       <c r="E19" s="9"/>
@@ -1378,13 +1378,13 @@
     </row>
     <row r="20" spans="1:12" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="9"/>
@@ -1400,13 +1400,13 @@
     </row>
     <row r="21" spans="1:12" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D21" s="16"/>
       <c r="E21" s="9"/>
@@ -1422,13 +1422,13 @@
     </row>
     <row r="22" spans="1:12" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D22" s="16"/>
       <c r="E22" s="9"/>
@@ -1444,13 +1444,13 @@
     </row>
     <row r="23" spans="1:12" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D23" s="16"/>
       <c r="E23" s="9"/>
@@ -1466,13 +1466,13 @@
     </row>
     <row r="24" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D24" s="25"/>
       <c r="E24" s="26"/>
@@ -1486,13 +1486,13 @@
     </row>
     <row r="25" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="9"/>
@@ -1508,13 +1508,13 @@
     </row>
     <row r="26" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D26" s="16"/>
       <c r="E26" s="9"/>
@@ -1530,13 +1530,13 @@
     </row>
     <row r="27" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D27" s="16"/>
       <c r="E27" s="9"/>
@@ -1552,13 +1552,13 @@
     </row>
     <row r="28" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="9"/>
@@ -1574,13 +1574,13 @@
     </row>
     <row r="29" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="9"/>
@@ -1596,13 +1596,13 @@
     </row>
     <row r="30" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D30" s="16"/>
       <c r="E30" s="9"/>
@@ -1618,13 +1618,13 @@
     </row>
     <row r="31" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D31" s="25"/>
       <c r="E31" s="26"/>
@@ -1638,13 +1638,13 @@
     </row>
     <row r="32" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D32" s="16"/>
       <c r="E32" s="9"/>
@@ -1660,13 +1660,13 @@
     </row>
     <row r="33" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D33" s="16"/>
       <c r="E33" s="9"/>
@@ -1682,13 +1682,13 @@
     </row>
     <row r="34" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D34" s="16"/>
       <c r="E34" s="9"/>
@@ -1704,13 +1704,13 @@
     </row>
     <row r="35" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D35" s="16"/>
       <c r="E35" s="9"/>
@@ -1726,13 +1726,13 @@
     </row>
     <row r="36" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="9"/>
@@ -1748,13 +1748,13 @@
     </row>
     <row r="37" spans="1:12" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D37" s="16"/>
       <c r="E37" s="9"/>
@@ -1773,10 +1773,10 @@
         <v>17</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D38" s="16"/>
       <c r="E38" s="9"/>
@@ -1793,10 +1793,10 @@
         <v>17</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="9"/>
@@ -1813,7 +1813,7 @@
         <v>18</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C40" s="20"/>
       <c r="D40" s="20"/>
@@ -1831,7 +1831,7 @@
         <v>19</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C41" s="20"/>
       <c r="D41" s="20"/>
@@ -1869,7 +1869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2:B12"/>
     </sheetView>
@@ -1903,51 +1903,51 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>25</v>
@@ -1958,7 +1958,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>26</v>
@@ -1972,13 +1972,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1986,46 +1986,46 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2539,8 +2539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2565,7 +2565,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>

</xml_diff>